<commit_message>
Kevins tests carried out
extra notes added under friends advice
</commit_message>
<xml_diff>
--- a/Pizza combinations, Kevin O'Hare.xlsx
+++ b/Pizza combinations, Kevin O'Hare.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="10">
   <si>
     <t>Olives</t>
   </si>
@@ -34,6 +34,18 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No, 9.39</t>
+  </si>
+  <si>
+    <t>No, 9.89</t>
+  </si>
+  <si>
+    <t>No, 10.39</t>
   </si>
 </sst>
 </file>
@@ -375,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,6 +658,56 @@
       </c>
       <c r="Q5" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>